<commit_message>
Update Corporate Finance Entire Worksheet.xlsx
</commit_message>
<xml_diff>
--- a/Corporate Finance/Corporate Finance Entire Worksheet.xlsx
+++ b/Corporate Finance/Corporate Finance Entire Worksheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hudac-my.sharepoint.com/personal/u2281887_unimail_hud_ac_uk/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ubayd\Documents\GitHub\University-Resources\Corporate Finance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1389" documentId="8_{746C739E-1B8A-4857-810C-E42BA09710FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{70808650-FBF6-E440-AC6F-AD7168AB32A7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9C2B456-339B-4397-8489-FA7514D28F84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2760" yWindow="500" windowWidth="31260" windowHeight="19640" firstSheet="7" activeTab="10" xr2:uid="{04150659-CC8A-470D-AA52-24A162A067B3}"/>
+    <workbookView xWindow="9195" yWindow="0" windowWidth="19710" windowHeight="15585" firstSheet="9" activeTab="11" xr2:uid="{04150659-CC8A-470D-AA52-24A162A067B3}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1 - Investment Appraisal" sheetId="1" r:id="rId1"/>
@@ -24,9 +24,9 @@
     <sheet name="Week 9 - Mergers" sheetId="9" r:id="rId9"/>
     <sheet name="Week 10 - Mergers II" sheetId="10" r:id="rId10"/>
     <sheet name="Past Exam Paper I" sheetId="12" r:id="rId11"/>
+    <sheet name="Week 14- Value Based Management" sheetId="13" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="517">
   <si>
     <t>Question 1)</t>
   </si>
@@ -1560,18 +1560,259 @@
   <si>
     <t>t is equal to the amount of years in question</t>
   </si>
+  <si>
+    <t>Question 1:</t>
+  </si>
+  <si>
+    <t>Sity plc has paid out all earnings as dividends since</t>
+  </si>
+  <si>
+    <t>it was founded with £15m of equity finance 25 years</t>
+  </si>
+  <si>
+    <t>ago. Today, its shares are valued on the stock market</t>
+  </si>
+  <si>
+    <t>at £90m and its long-term debt has a market value</t>
+  </si>
+  <si>
+    <t>and book value of £20m.</t>
+  </si>
+  <si>
+    <t>a] How much market value added (MVA) has Sity</t>
+  </si>
+  <si>
+    <t>produced?</t>
+  </si>
+  <si>
+    <t>b] What is Sity's market-to-book ratio (MBR)?</t>
+  </si>
+  <si>
+    <t>c] Given that another company, Pity plc, was founded</t>
+  </si>
+  <si>
+    <t>with £15m of equity capital five years ago and has paid</t>
+  </si>
+  <si>
+    <t>out all earnings since its foundation and is now worth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(equity and debt) £110m (£90m equity, £20m debt), </t>
+  </si>
+  <si>
+    <t>discuss the problems of using the MVA and the MB for</t>
+  </si>
+  <si>
+    <t>inter-firm comparison.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d] Calculate the excess return (ER) for both Sity and </t>
+  </si>
+  <si>
+    <t>Pity, given that the required rate of reutrn for Sity is</t>
+  </si>
+  <si>
+    <t>8 per cent per year and the required rate of return is</t>
+  </si>
+  <si>
+    <t>10 per cent per year for Pity. Sity has paid only two</t>
+  </si>
+  <si>
+    <t>dividends: £2m was paid five years ago and £3m was</t>
+  </si>
+  <si>
+    <t>paid three years ago. Pity has paid £2m in dividends</t>
+  </si>
+  <si>
+    <t>at the end of every year since its foundation.</t>
+  </si>
+  <si>
+    <t>Market Value Added = Current Share Value</t>
+  </si>
+  <si>
+    <t>- Original Capital</t>
+  </si>
+  <si>
+    <t>Current Share Value</t>
+  </si>
+  <si>
+    <t>Original Capital</t>
+  </si>
+  <si>
+    <t>Value Added</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Market Value added = </t>
+  </si>
+  <si>
+    <t>Formula Required:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Market-to-book ratio = </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 90/15 = 6</t>
+  </si>
+  <si>
+    <t>It's essential in this case to compare the nature and</t>
+  </si>
+  <si>
+    <t>industries of both companies, as they can possess</t>
+  </si>
+  <si>
+    <t xml:space="preserve">differing capital intensity, growth rates, as well as </t>
+  </si>
+  <si>
+    <t xml:space="preserve">risk profiles. </t>
+  </si>
+  <si>
+    <t>For example, comparing a tech startup with a utility</t>
+  </si>
+  <si>
+    <t>company using MVA or MBR is highly likely to become</t>
+  </si>
+  <si>
+    <t xml:space="preserve">misleading. This is due to tech companies often </t>
+  </si>
+  <si>
+    <t>possessing higher MBs due to growth potential.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As neither of their industries are specified, the </t>
+  </si>
+  <si>
+    <t>comparisons between both would become difficult,</t>
+  </si>
+  <si>
+    <t>especially when disregarding industry benchmarks.</t>
+  </si>
+  <si>
+    <t>Furthermore, larger and more established companies</t>
+  </si>
+  <si>
+    <t>more often have higher MVAs simply due to their scale.</t>
+  </si>
+  <si>
+    <t>Smaller, more quickly growing companies could have</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lower MVAs despite possessing higher MBRs, which </t>
+  </si>
+  <si>
+    <t>would indicate a better long-term potential.</t>
+  </si>
+  <si>
+    <t>Therefore with Pity plc being 5 years old, the natures of</t>
+  </si>
+  <si>
+    <t>both comparisons being too different is likely to invalidate</t>
+  </si>
+  <si>
+    <t>any meanings of the results obtained from inter-firm</t>
+  </si>
+  <si>
+    <t>comparison of MVA and MBR.</t>
+  </si>
+  <si>
+    <t>Actual Wealth</t>
+  </si>
+  <si>
+    <t>Dividend</t>
+  </si>
+  <si>
+    <t>Formula of PV</t>
+  </si>
+  <si>
+    <t>Dividend 1</t>
+  </si>
+  <si>
+    <t>Dividend 2</t>
+  </si>
+  <si>
+    <t>Value of Shares</t>
+  </si>
+  <si>
+    <t>Total Value</t>
+  </si>
+  <si>
+    <t>5 Y</t>
+  </si>
+  <si>
+    <t>3 Y</t>
+  </si>
+  <si>
+    <t>2 mil</t>
+  </si>
+  <si>
+    <t>3 mil</t>
+  </si>
+  <si>
+    <t>2(1.08)^5</t>
+  </si>
+  <si>
+    <t>2(1.08)^3</t>
+  </si>
+  <si>
+    <t>= 3.779 mil</t>
+  </si>
+  <si>
+    <t>= 2.939 mil</t>
+  </si>
+  <si>
+    <t>= 90 mil</t>
+  </si>
+  <si>
+    <t>= 96.718 mil</t>
+  </si>
+  <si>
+    <t>Expected Wealth:</t>
+  </si>
+  <si>
+    <t>15(1.08)^25 = 102.727 mil</t>
+  </si>
+  <si>
+    <t>Excess Return:</t>
+  </si>
+  <si>
+    <t>96.718 mil - 102.727 mil = -6.01 mil</t>
+  </si>
+  <si>
+    <t>Sity Company</t>
+  </si>
+  <si>
+    <t>Pity Company</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Each </t>
+  </si>
+  <si>
+    <t>2*6.1051</t>
+  </si>
+  <si>
+    <t>= 12.21 mil</t>
+  </si>
+  <si>
+    <t>= 102.21 mil</t>
+  </si>
+  <si>
+    <t>15(1.1)^5 = 24.15 mil</t>
+  </si>
+  <si>
+    <t>102.21 mil - 24.15 mil = 78.06 mil</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="6">
-    <numFmt numFmtId="6" formatCode="&quot;£&quot;#,##0_);[Red]\(&quot;£&quot;#,##0\)"/>
-    <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00_);[Red]\(&quot;£&quot;#,##0.00\)"/>
-    <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
-    <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="#,##0.000"/>
-    <numFmt numFmtId="167" formatCode="&quot;£&quot;#,##0.0_);[Red]\(&quot;£&quot;#,##0.0\)"/>
+  <numFmts count="7">
+    <numFmt numFmtId="6" formatCode="&quot;£&quot;#,##0;[Red]\-&quot;£&quot;#,##0"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0_);[Red]\(&quot;£&quot;#,##0\)"/>
+    <numFmt numFmtId="165" formatCode="&quot;£&quot;#,##0.00_);[Red]\(&quot;£&quot;#,##0.00\)"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="#,##0.000"/>
+    <numFmt numFmtId="168" formatCode="&quot;£&quot;#,##0.0_);[Red]\(&quot;£&quot;#,##0.0\)"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -1826,7 +2067,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1837,10 +2078,10 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -1849,7 +2090,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1863,39 +2104,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="6" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="6" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="8" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4005,10 +4248,6 @@
 </inkml:ink>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -4332,81 +4571,81 @@
       <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I3" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I5" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I6" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I7" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I9" s="1">
         <f>146.41 + 266.2 + 242 + 330 + 300</f>
         <v>1284.6100000000001</v>
       </c>
     </row>
-    <row r="12" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I12" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I13" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I14" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="9:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="9:9" x14ac:dyDescent="0.25">
       <c r="I15">
         <f xml:space="preserve"> 292.82 + 605 + 300</f>
         <v>1197.82</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I17" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I18" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I20" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>17</v>
       </c>
@@ -4414,7 +4653,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>18</v>
       </c>
@@ -4422,7 +4661,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -4430,12 +4669,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I25" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>10</v>
       </c>
@@ -4447,7 +4686,7 @@
         <v>710.04</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>22</v>
       </c>
@@ -4455,7 +4694,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>20</v>
       </c>
@@ -4466,7 +4705,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>21</v>
       </c>
@@ -4477,7 +4716,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <f xml:space="preserve"> 100 * 6.7424</f>
         <v>674.24</v>
@@ -4490,13 +4729,13 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I31" s="1">
         <f>175.44 + 337.49 + 155.81</f>
         <v>668.74</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>23</v>
       </c>
@@ -4504,7 +4743,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>24</v>
       </c>
@@ -4515,7 +4754,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>25</v>
       </c>
@@ -4526,7 +4765,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <f xml:space="preserve"> 300 * 6.7424</f>
         <v>2022.72</v>
@@ -4536,22 +4775,22 @@
         <v>1005.66</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>33</v>
       </c>
@@ -4564,7 +4803,7 @@
       <c r="H42" s="5"/>
       <c r="I42" s="5"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>34</v>
       </c>
@@ -4577,7 +4816,7 @@
       <c r="H43" s="5"/>
       <c r="I43" s="5"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>35</v>
       </c>
@@ -4590,7 +4829,7 @@
       <c r="H44" s="5"/>
       <c r="I44" s="5"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>36</v>
       </c>
@@ -4603,7 +4842,7 @@
       <c r="H45" s="5"/>
       <c r="I45" s="5"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>37</v>
       </c>
@@ -4616,7 +4855,7 @@
       <c r="H46" s="5"/>
       <c r="I46" s="5"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>38</v>
       </c>
@@ -4629,7 +4868,7 @@
       <c r="H47" s="5"/>
       <c r="I47" s="5"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>39</v>
       </c>
@@ -4642,7 +4881,7 @@
       <c r="H48" s="5"/>
       <c r="I48" s="5"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>40</v>
       </c>
@@ -4655,7 +4894,7 @@
       <c r="H49" s="5"/>
       <c r="I49" s="5"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>41</v>
       </c>
@@ -4668,7 +4907,7 @@
       <c r="H50" s="5"/>
       <c r="I50" s="5"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>42</v>
       </c>
@@ -4681,7 +4920,7 @@
       <c r="H51" s="5"/>
       <c r="I51" s="5"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>43</v>
       </c>
@@ -4694,7 +4933,7 @@
       <c r="H52" s="5"/>
       <c r="I52" s="5"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>44</v>
       </c>
@@ -4707,7 +4946,7 @@
       <c r="H53" s="5"/>
       <c r="I53" s="5"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>45</v>
       </c>
@@ -4720,7 +4959,7 @@
       <c r="H54" s="5"/>
       <c r="I54" s="5"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>46</v>
       </c>
@@ -4733,7 +4972,7 @@
       <c r="H55" s="5"/>
       <c r="I55" s="5"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>47</v>
       </c>
@@ -4746,7 +4985,7 @@
       <c r="H56" s="5"/>
       <c r="I56" s="5"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>48</v>
       </c>
@@ -4759,7 +4998,7 @@
       <c r="H57" s="5"/>
       <c r="I57" s="5"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>49</v>
       </c>
@@ -4772,7 +5011,7 @@
       <c r="H58" s="5"/>
       <c r="I58" s="5"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>50</v>
       </c>
@@ -4785,7 +5024,7 @@
       <c r="H59" s="5"/>
       <c r="I59" s="5"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>51</v>
       </c>
@@ -4798,7 +5037,7 @@
       <c r="H60" s="5"/>
       <c r="I60" s="5"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>52</v>
       </c>
@@ -4811,7 +5050,7 @@
       <c r="H61" s="5"/>
       <c r="I61" s="5"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>53</v>
       </c>
@@ -4824,7 +5063,7 @@
       <c r="H62" s="5"/>
       <c r="I62" s="5"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>54</v>
       </c>
@@ -4837,7 +5076,7 @@
       <c r="H63" s="5"/>
       <c r="I63" s="5"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>55</v>
       </c>
@@ -4850,7 +5089,7 @@
       <c r="H64" s="5"/>
       <c r="I64" s="5"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>56</v>
       </c>
@@ -4863,7 +5102,7 @@
       <c r="H65" s="5"/>
       <c r="I65" s="5"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="6"/>
     </row>
   </sheetData>
@@ -4880,9 +5119,9 @@
       <selection activeCell="H67" sqref="H66:H67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>17</v>
       </c>
@@ -4890,7 +5129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>380</v>
       </c>
@@ -4898,22 +5137,22 @@
         <v>348</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I5" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I7" s="2" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>379</v>
       </c>
@@ -4921,7 +5160,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>377</v>
       </c>
@@ -4929,22 +5168,22 @@
         <v>352</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I10" s="1" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I12" s="2" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>375</v>
       </c>
@@ -4952,7 +5191,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>376</v>
       </c>
@@ -4960,7 +5199,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>381</v>
       </c>
@@ -4968,7 +5207,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>382</v>
       </c>
@@ -4976,7 +5215,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>383</v>
       </c>
@@ -4984,7 +5223,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
         <v>387</v>
       </c>
@@ -4992,17 +5231,17 @@
         <v>359</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I24" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>385</v>
       </c>
@@ -5010,32 +5249,32 @@
         <v>361</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I27" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I29" s="2" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I31" s="1" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
         <v>389</v>
       </c>
@@ -5043,7 +5282,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>390</v>
       </c>
@@ -5051,7 +5290,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>391</v>
       </c>
@@ -5059,17 +5298,17 @@
         <v>366</v>
       </c>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I40" s="2" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>393</v>
       </c>
@@ -5077,17 +5316,17 @@
         <v>368</v>
       </c>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="I43" s="2" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>395</v>
       </c>
@@ -5095,7 +5334,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>396</v>
       </c>
@@ -5103,7 +5342,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>397</v>
       </c>
@@ -5112,7 +5351,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" s="1" t="s">
         <v>398</v>
       </c>
@@ -5126,485 +5365,486 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{002F2DCF-F2C8-1A4D-BC9A-EFBCE1ECAC1F}">
   <dimension ref="A3:L61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="147" zoomScaleNormal="147" workbookViewId="0">
+    <sheetView topLeftCell="A31" zoomScale="145" zoomScaleNormal="147" workbookViewId="0">
       <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="48"/>
-    <col min="2" max="2" width="13.33203125" style="48" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="12.5" style="48" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="48"/>
+    <col min="1" max="1" width="10.85546875" style="43"/>
+    <col min="2" max="2" width="13.42578125" style="43" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.5703125" style="43" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="43" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.85546875" style="43"/>
   </cols>
   <sheetData>
-    <row r="3" spans="7:12" x14ac:dyDescent="0.2">
-      <c r="G3" s="50" t="s">
+    <row r="3" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G3" s="45" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="4" spans="7:12" x14ac:dyDescent="0.2">
-      <c r="G4" s="50" t="s">
+    <row r="4" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G4" s="45" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="6" spans="7:12" x14ac:dyDescent="0.2">
-      <c r="G6" s="50" t="s">
+    <row r="6" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G6" s="45" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="8" spans="7:12" x14ac:dyDescent="0.2">
-      <c r="G8" s="50" t="s">
+    <row r="8" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G8" s="45" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="9" spans="7:12" x14ac:dyDescent="0.2">
-      <c r="G9" s="49" t="s">
+    <row r="9" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G9" s="44" t="s">
         <v>403</v>
       </c>
-      <c r="L9" s="50" t="s">
+      <c r="L9" s="45" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="10" spans="7:12" x14ac:dyDescent="0.2">
-      <c r="G10" s="49" t="s">
+    <row r="10" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G10" s="44" t="s">
         <v>404</v>
       </c>
-      <c r="L10" s="50" t="s">
+      <c r="L10" s="45" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="11" spans="7:12" x14ac:dyDescent="0.2">
-      <c r="G11" s="49" t="s">
+    <row r="11" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G11" s="44" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="13" spans="7:12" x14ac:dyDescent="0.2">
-      <c r="G13" s="50" t="s">
+    <row r="13" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G13" s="45" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="14" spans="7:12" x14ac:dyDescent="0.2">
-      <c r="G14" s="48" t="s">
+    <row r="14" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G14" s="43" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="16" spans="7:12" x14ac:dyDescent="0.2">
-      <c r="G16" s="48" t="s">
+    <row r="16" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G16" s="43" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G17" s="48" t="s">
+    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G17" s="43" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G18" s="49" t="s">
+    <row r="18" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G18" s="44" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="21" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G21" s="50" t="s">
+    <row r="21" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G21" s="45" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="23" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G23" s="50" t="s">
+    <row r="23" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G23" s="45" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="24" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G24" s="49" t="s">
+    <row r="24" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G24" s="44" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="25" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G25" s="49" t="s">
+    <row r="25" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G25" s="44" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="26" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G26" s="49" t="s">
+    <row r="26" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G26" s="44" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="27" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G27" s="49" t="s">
+    <row r="27" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G27" s="44" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="50" t="s">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="45" t="s">
         <v>415</v>
       </c>
-      <c r="G34" s="50" t="s">
+      <c r="G34" s="45" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="50" t="s">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="45" t="s">
         <v>416</v>
       </c>
-      <c r="G35" s="50" t="s">
+      <c r="G35" s="45" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B37" s="50" t="s">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B37" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="C37" s="50" t="s">
+      <c r="C37" s="45" t="s">
         <v>61</v>
       </c>
-      <c r="D37" s="50" t="s">
+      <c r="D37" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="E37" s="50" t="s">
+      <c r="E37" s="45" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" s="54" t="s">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="43" t="s">
         <v>417</v>
       </c>
-      <c r="B38" s="48">
+      <c r="B38" s="43">
         <v>800000</v>
       </c>
-      <c r="C38" s="48">
+      <c r="C38" s="43">
         <v>900000</v>
       </c>
-      <c r="D38" s="48">
+      <c r="D38" s="43">
         <v>1000000</v>
       </c>
-      <c r="E38" s="48">
+      <c r="E38" s="43">
         <v>1100000</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" s="50" t="s">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="45" t="s">
         <v>108</v>
       </c>
-      <c r="B39" s="51">
+      <c r="B39" s="46">
         <f>10*B38</f>
         <v>8000000</v>
       </c>
-      <c r="C39" s="48">
+      <c r="C39" s="43">
         <f>10.4*C38</f>
         <v>9360000</v>
       </c>
-      <c r="D39" s="48">
+      <c r="D39" s="43">
         <f>10.816*D38</f>
         <v>10816000</v>
       </c>
-      <c r="E39" s="48">
+      <c r="E39" s="43">
         <f>11.2484*E38</f>
         <v>12373240</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" s="50" t="s">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="45" t="s">
         <v>418</v>
       </c>
-      <c r="B40" s="48">
+      <c r="B40" s="43">
         <f>3.5*B38</f>
         <v>2800000</v>
       </c>
-      <c r="C40" s="48">
+      <c r="C40" s="43">
         <f>(3.5*1.01)*C38</f>
         <v>3181500</v>
       </c>
-      <c r="D40" s="48">
+      <c r="D40" s="43">
         <f>(3.535*1.01)*D38</f>
         <v>3570350.0000000005</v>
       </c>
-      <c r="E40" s="48">
+      <c r="E40" s="43">
         <f>(3.5705*1.01)*E38</f>
         <v>3966825.5</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" s="50" t="s">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="45" t="s">
         <v>419</v>
       </c>
-      <c r="B41" s="48">
+      <c r="B41" s="43">
         <f>2*B38</f>
         <v>1600000</v>
       </c>
-      <c r="C41" s="48">
+      <c r="C41" s="43">
         <f>(2*1.05)*C38</f>
         <v>1890000</v>
       </c>
-      <c r="D41" s="48">
+      <c r="D41" s="43">
         <f>(2*(1.05+0.05))*D38</f>
         <v>2200000</v>
       </c>
-      <c r="E41" s="48">
+      <c r="E41" s="43">
         <f>(2*(1.05+0.05+0.05))*E38</f>
         <v>2530000.0000000005</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A42" s="50" t="s">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="45" t="s">
         <v>420</v>
       </c>
-      <c r="B42" s="48">
+      <c r="B42" s="43">
         <f>450000-125000</f>
         <v>325000</v>
       </c>
-      <c r="C42" s="48">
+      <c r="C42" s="43">
         <f>B42*1.03</f>
         <v>334750</v>
       </c>
-      <c r="D42" s="48">
+      <c r="D42" s="43">
         <f>C42*1.03</f>
         <v>344792.5</v>
       </c>
-      <c r="E42" s="48">
+      <c r="E42" s="43">
         <f>D42*1.03</f>
         <v>355136.27500000002</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B45" s="50" t="s">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B45" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="C45" s="50" t="s">
+      <c r="C45" s="45" t="s">
         <v>61</v>
       </c>
-      <c r="D45" s="50" t="s">
+      <c r="D45" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="E45" s="50" t="s">
+      <c r="E45" s="45" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46" s="50" t="s">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="B46" s="51">
+      <c r="B46" s="46">
         <f>B39-B40-B41-B42</f>
         <v>3275000</v>
       </c>
-      <c r="C46" s="51">
+      <c r="C46" s="46">
         <f t="shared" ref="C46:E46" si="0">C39-C40-C41-C42</f>
         <v>3953750</v>
       </c>
-      <c r="D46" s="51">
+      <c r="D46" s="46">
         <f t="shared" si="0"/>
         <v>4700857.5</v>
       </c>
-      <c r="E46" s="51">
+      <c r="E46" s="46">
         <f t="shared" si="0"/>
         <v>5521278.2249999996</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A47" s="50" t="s">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="45" t="s">
         <v>422</v>
       </c>
-      <c r="B47" s="48">
+      <c r="B47" s="43">
         <f>0.25*9500000</f>
         <v>2375000</v>
       </c>
-      <c r="C47" s="48">
+      <c r="C47" s="43">
         <f>B47*0.75</f>
         <v>1781250</v>
       </c>
-      <c r="D47" s="48">
+      <c r="D47" s="43">
         <f>C47*0.75</f>
         <v>1335937.5</v>
       </c>
-      <c r="E47" s="52">
+      <c r="E47" s="47">
         <f>D47*0.75+(0.25*E46)</f>
         <v>2382272.6812499999</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A48" s="50" t="s">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="45" t="s">
         <v>421</v>
       </c>
-      <c r="B48" s="51">
+      <c r="B48" s="46">
         <f>B46-B47</f>
         <v>900000</v>
       </c>
-      <c r="C48" s="51">
+      <c r="C48" s="46">
         <f t="shared" ref="C48:E48" si="1">C46-C47</f>
         <v>2172500</v>
       </c>
-      <c r="D48" s="51">
+      <c r="D48" s="46">
         <f t="shared" si="1"/>
         <v>3364920</v>
       </c>
-      <c r="E48" s="51">
+      <c r="E48" s="46">
         <f t="shared" si="1"/>
         <v>3139005.5437499997</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A49" s="50" t="s">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="45" t="s">
         <v>132</v>
       </c>
-      <c r="B49" s="53">
+      <c r="B49" s="48">
         <f>(0.2*B48)</f>
         <v>180000</v>
       </c>
-      <c r="C49" s="53">
+      <c r="C49" s="48">
         <f t="shared" ref="C49:E49" si="2">(0.2*C48)</f>
         <v>434500</v>
       </c>
-      <c r="D49" s="53">
+      <c r="D49" s="48">
         <f t="shared" si="2"/>
         <v>672984</v>
       </c>
-      <c r="E49" s="53">
+      <c r="E49" s="48">
         <f t="shared" si="2"/>
         <v>627801.10875000001</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B52" s="50" t="s">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B52" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="C52" s="50" t="s">
+      <c r="C52" s="45" t="s">
         <v>61</v>
       </c>
-      <c r="D52" s="50" t="s">
+      <c r="D52" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="E52" s="50" t="s">
+      <c r="E52" s="45" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A53" s="50" t="s">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="B53" s="51">
+      <c r="B53" s="46">
         <f>B46-B49</f>
         <v>3095000</v>
       </c>
-      <c r="C53" s="51">
+      <c r="C53" s="46">
         <f t="shared" ref="C53:D53" si="3">C46-C49</f>
         <v>3519250</v>
       </c>
-      <c r="D53" s="51">
+      <c r="D53" s="46">
         <f t="shared" si="3"/>
         <v>4027873.5</v>
       </c>
-      <c r="E53" s="51">
+      <c r="E53" s="46">
         <f>E46-E49</f>
         <v>4893477.11625</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A54" s="50" t="s">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="45" t="s">
         <v>423</v>
       </c>
-      <c r="E54" s="52">
+      <c r="E54" s="47">
         <v>1375000</v>
       </c>
-      <c r="G54" s="50" t="s">
+      <c r="G54" s="45" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A55" s="50" t="s">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="45" t="s">
         <v>424</v>
       </c>
-      <c r="B55" s="51">
+      <c r="B55" s="46">
         <f>B53-B54</f>
         <v>3095000</v>
       </c>
-      <c r="C55" s="51">
-        <f t="shared" ref="C55:E55" si="4">C53-C54</f>
+      <c r="C55" s="46">
+        <f t="shared" ref="C55:D55" si="4">C53-C54</f>
         <v>3519250</v>
       </c>
-      <c r="D55" s="51">
+      <c r="D55" s="46">
         <f t="shared" si="4"/>
         <v>4027873.5</v>
       </c>
-      <c r="E55" s="51">
+      <c r="E55" s="46">
         <f>E53+E54</f>
         <v>6268477.11625</v>
       </c>
-      <c r="G55" s="48" t="s">
+      <c r="G55" s="43" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A56" s="50" t="s">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="45" t="s">
         <v>425</v>
       </c>
-      <c r="B56" s="48">
+      <c r="B56" s="43">
         <f>1/(1+0.11)^1</f>
         <v>0.9009009009009008</v>
       </c>
-      <c r="C56" s="48">
+      <c r="C56" s="43">
         <f>1/(1+0.11)^2</f>
         <v>0.8116224332440547</v>
       </c>
-      <c r="D56" s="48">
+      <c r="D56" s="43">
         <f>1/(1+0.11)^3</f>
         <v>0.73119138130095018</v>
       </c>
-      <c r="E56" s="48">
+      <c r="E56" s="43">
         <f>1/(1+0.11)^4</f>
         <v>0.65873097414500015</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A57" s="50" t="s">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="45" t="s">
         <v>426</v>
       </c>
-      <c r="B57" s="52">
+      <c r="B57" s="47">
         <f>B55*B56</f>
         <v>2788288.2882882878</v>
       </c>
-      <c r="C57" s="52">
+      <c r="C57" s="47">
         <f t="shared" ref="C57:E57" si="5">C55*C56</f>
         <v>2856302.2481941395</v>
       </c>
-      <c r="D57" s="52">
+      <c r="D57" s="47">
         <f t="shared" si="5"/>
         <v>2945146.3881704928</v>
       </c>
-      <c r="E57" s="52">
+      <c r="E57" s="47">
         <f t="shared" si="5"/>
         <v>4129240.037193004</v>
       </c>
-      <c r="G57" s="48" t="s">
+      <c r="G57" s="43" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="G58" s="48" t="s">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G58" s="43" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A59" s="50" t="s">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="45" t="s">
         <v>427</v>
       </c>
-      <c r="B59" s="52">
+      <c r="B59" s="47">
         <f>B57+C57+D57+E57</f>
         <v>12718976.961845923</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A60" s="50" t="s">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="45" t="s">
         <v>117</v>
       </c>
-      <c r="B60" s="51">
+      <c r="B60" s="46">
         <v>9500000</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A61" s="50" t="s">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="B61" s="52">
+      <c r="B61" s="47">
         <f>B59-B60</f>
         <v>3218976.9618459232</v>
       </c>
@@ -5613,6 +5853,416 @@
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B57FBCE-DA46-4952-8AAA-B3F9ED31A3BE}">
+  <dimension ref="C2:U46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E12" workbookViewId="0">
+      <selection activeCell="O18" sqref="O18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C2" s="42" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="4" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="5" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="6" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="7" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="8" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="10" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C10" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="11" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C11" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="12" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="I12" s="55" t="s">
+        <v>466</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="13" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C13" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="I13" s="56" t="s">
+        <v>467</v>
+      </c>
+      <c r="O13" s="2" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="14" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="O14" s="2" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="15" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>459</v>
+      </c>
+      <c r="O15" s="2" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="16" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C16" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="O16" s="2" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="17" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="I17" s="2" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="18" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>461</v>
+      </c>
+      <c r="F18">
+        <f>90</f>
+        <v>90</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="O18" s="42" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="19" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C19" s="9" t="s">
+        <v>462</v>
+      </c>
+      <c r="D19" s="9"/>
+      <c r="F19" s="9">
+        <f>-15</f>
+        <v>-15</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="20" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C20" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2">
+        <f>F18+F19</f>
+        <v>75</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="O20" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="R20" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="S20" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="T20" s="2"/>
+      <c r="U20" s="2" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="21" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="I21" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="O21" s="55" t="s">
+        <v>491</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>495</v>
+      </c>
+      <c r="R21" t="s">
+        <v>497</v>
+      </c>
+      <c r="S21" t="s">
+        <v>499</v>
+      </c>
+      <c r="U21" s="1" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="22" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C22" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="54">
+        <f>F20*1000000</f>
+        <v>75000000</v>
+      </c>
+      <c r="O22" s="55" t="s">
+        <v>492</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>496</v>
+      </c>
+      <c r="R22" t="s">
+        <v>498</v>
+      </c>
+      <c r="S22" t="s">
+        <v>500</v>
+      </c>
+      <c r="U22" s="1" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="23" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="I23" t="s">
+        <v>468</v>
+      </c>
+      <c r="O23" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="U23" s="1" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="24" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="I24" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="25" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="I25" t="s">
+        <v>470</v>
+      </c>
+      <c r="O25" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="U25" s="1" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="26" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="I26" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="27" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="O27" s="2" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="28" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="I28" t="s">
+        <v>472</v>
+      </c>
+      <c r="O28" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="29" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="I29" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="30" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="I30" t="s">
+        <v>474</v>
+      </c>
+      <c r="O30" s="2" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="31" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="I31" t="s">
+        <v>475</v>
+      </c>
+      <c r="O31" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="33" spans="9:21" x14ac:dyDescent="0.25">
+      <c r="I33" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="34" spans="9:21" x14ac:dyDescent="0.25">
+      <c r="I34" t="s">
+        <v>477</v>
+      </c>
+      <c r="O34" s="42" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="35" spans="9:21" x14ac:dyDescent="0.25">
+      <c r="I35" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="36" spans="9:21" x14ac:dyDescent="0.25">
+      <c r="O36" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="P36" s="2"/>
+      <c r="Q36" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="R36" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="S36" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="T36" s="2"/>
+      <c r="U36" s="2" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="37" spans="9:21" x14ac:dyDescent="0.25">
+      <c r="I37" t="s">
+        <v>479</v>
+      </c>
+      <c r="O37" t="s">
+        <v>489</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>511</v>
+      </c>
+      <c r="R37" t="s">
+        <v>497</v>
+      </c>
+      <c r="S37" t="s">
+        <v>512</v>
+      </c>
+      <c r="U37" s="1" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="38" spans="9:21" x14ac:dyDescent="0.25">
+      <c r="I38" t="s">
+        <v>480</v>
+      </c>
+      <c r="O38" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="U38" s="1" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="39" spans="9:21" x14ac:dyDescent="0.25">
+      <c r="I39" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="40" spans="9:21" x14ac:dyDescent="0.25">
+      <c r="I40" t="s">
+        <v>482</v>
+      </c>
+      <c r="O40" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="U40" s="1" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="41" spans="9:21" x14ac:dyDescent="0.25">
+      <c r="I41" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="42" spans="9:21" x14ac:dyDescent="0.25">
+      <c r="O42" s="2" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="43" spans="9:21" x14ac:dyDescent="0.25">
+      <c r="I43" t="s">
+        <v>484</v>
+      </c>
+      <c r="O43" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="44" spans="9:21" x14ac:dyDescent="0.25">
+      <c r="I44" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="45" spans="9:21" x14ac:dyDescent="0.25">
+      <c r="I45" t="s">
+        <v>486</v>
+      </c>
+      <c r="O45" s="2" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="46" spans="9:21" x14ac:dyDescent="0.25">
+      <c r="I46" t="s">
+        <v>487</v>
+      </c>
+      <c r="O46" t="s">
+        <v>516</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -5624,21 +6274,21 @@
       <selection activeCell="L40" sqref="L40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5" customWidth="1"/>
-    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="10" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J1" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J3" t="s">
         <v>59</v>
       </c>
@@ -5650,7 +6300,7 @@
         <v>-600000</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J4" t="s">
         <v>60</v>
       </c>
@@ -5662,7 +6312,7 @@
         <v>-425000</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J5" t="s">
         <v>61</v>
       </c>
@@ -5674,7 +6324,7 @@
         <v>-250000</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J6" t="s">
         <v>62</v>
       </c>
@@ -5686,7 +6336,7 @@
         <v>-75000</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J7" t="s">
         <v>63</v>
       </c>
@@ -5698,22 +6348,22 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J9" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J10" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J13" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="J15" t="s">
         <v>59</v>
       </c>
@@ -5725,7 +6375,7 @@
         <v>-500000</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>79</v>
       </c>
@@ -5743,7 +6393,7 @@
         <v>-325000</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="J17" t="s">
         <v>61</v>
       </c>
@@ -5755,7 +6405,7 @@
         <v>-150000</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>69</v>
       </c>
@@ -5791,7 +6441,7 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>59</v>
       </c>
@@ -5819,7 +6469,7 @@
         <v>-500000</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>80</v>
       </c>
@@ -5850,7 +6500,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>76</v>
       </c>
@@ -5881,7 +6531,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="C22" s="2" t="s">
         <v>77</v>
       </c>
@@ -5897,7 +6547,7 @@
         <v>-35405</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="J24" s="2" t="s">
         <v>68</v>
       </c>
@@ -5905,7 +6555,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="J26" s="2" t="s">
         <v>69</v>
       </c>
@@ -5931,7 +6581,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="J27" t="s">
         <v>59</v>
       </c>
@@ -5958,7 +6608,7 @@
         <v>-500000</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="J28" t="s">
         <v>60</v>
       </c>
@@ -5986,7 +6636,7 @@
         <v>156625</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="J29" t="s">
         <v>61</v>
       </c>
@@ -6014,7 +6664,7 @@
         <v>139475</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>11</v>
       </c>
@@ -6045,7 +6695,7 @@
         <v>124600</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="J31" t="s">
         <v>63</v>
       </c>
@@ -6073,7 +6723,7 @@
         <v>111300</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>84</v>
       </c>
@@ -6104,7 +6754,7 @@
         <v>99224.999999999985</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>85</v>
       </c>
@@ -6135,7 +6785,7 @@
         <v>93795</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>86</v>
       </c>
@@ -6160,7 +6810,7 @@
         <v>225020</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="J35" t="s">
         <v>76</v>
       </c>
@@ -6175,7 +6825,7 @@
         <v>90900</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="11"/>
       <c r="B36" s="12" t="s">
         <v>89</v>
@@ -6194,7 +6844,7 @@
         <v>289950</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
         <v>87</v>
       </c>
@@ -6208,7 +6858,7 @@
         <v>0.24610000000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>88</v>
       </c>
@@ -6222,62 +6872,62 @@
         <v>0.27550000000000002</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>104</v>
       </c>
@@ -6298,14 +6948,14 @@
       <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="10:22" x14ac:dyDescent="0.2">
+    <row r="2" spans="10:22" x14ac:dyDescent="0.25">
       <c r="J2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="10:22" x14ac:dyDescent="0.2">
+    <row r="4" spans="10:22" x14ac:dyDescent="0.25">
       <c r="J4" t="s">
         <v>106</v>
       </c>
@@ -6313,23 +6963,23 @@
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="10:22" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J6" s="45" t="s">
+    <row r="6" spans="10:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J6" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="K6" s="45"/>
-      <c r="L6" s="45"/>
-      <c r="M6" s="45"/>
-      <c r="Q6" s="45" t="s">
+      <c r="K6" s="49"/>
+      <c r="L6" s="49"/>
+      <c r="M6" s="49"/>
+      <c r="Q6" s="49" t="s">
         <v>132</v>
       </c>
-      <c r="R6" s="45"/>
-      <c r="S6" s="45"/>
-      <c r="T6" s="45"/>
-      <c r="U6" s="45"/>
-      <c r="V6" s="45"/>
-    </row>
-    <row r="7" spans="10:22" x14ac:dyDescent="0.2">
+      <c r="R6" s="49"/>
+      <c r="S6" s="49"/>
+      <c r="T6" s="49"/>
+      <c r="U6" s="49"/>
+      <c r="V6" s="49"/>
+    </row>
+    <row r="7" spans="10:22" x14ac:dyDescent="0.25">
       <c r="J7" t="s">
         <v>108</v>
       </c>
@@ -6349,7 +6999,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="10:22" x14ac:dyDescent="0.2">
+    <row r="8" spans="10:22" x14ac:dyDescent="0.25">
       <c r="J8" t="s">
         <v>109</v>
       </c>
@@ -6372,7 +7022,7 @@
         <v>55000</v>
       </c>
     </row>
-    <row r="9" spans="10:22" x14ac:dyDescent="0.2">
+    <row r="9" spans="10:22" x14ac:dyDescent="0.25">
       <c r="J9" t="s">
         <v>110</v>
       </c>
@@ -6399,25 +7049,25 @@
         <v>2687.5</v>
       </c>
     </row>
-    <row r="10" spans="10:22" x14ac:dyDescent="0.2">
+    <row r="10" spans="10:22" x14ac:dyDescent="0.25">
       <c r="J10" t="s">
         <v>111</v>
       </c>
       <c r="L10" s="16">
         <v>-20000</v>
       </c>
-      <c r="Q10" s="47" t="s">
+      <c r="Q10" s="50" t="s">
         <v>133</v>
       </c>
-      <c r="R10" s="47"/>
-    </row>
-    <row r="11" spans="10:22" x14ac:dyDescent="0.2">
+      <c r="R10" s="50"/>
+    </row>
+    <row r="11" spans="10:22" x14ac:dyDescent="0.25">
       <c r="L11" s="7">
         <f>SUM(L7:L10)</f>
         <v>55000</v>
       </c>
-      <c r="Q11" s="47"/>
-      <c r="R11" s="47"/>
+      <c r="Q11" s="50"/>
+      <c r="R11" s="50"/>
       <c r="S11" s="7">
         <f>S8+S9</f>
         <v>40000</v>
@@ -6435,10 +7085,10 @@
         <v>57687.5</v>
       </c>
     </row>
-    <row r="12" spans="10:22" x14ac:dyDescent="0.2">
+    <row r="12" spans="10:22" x14ac:dyDescent="0.25">
       <c r="Q12" s="2"/>
     </row>
-    <row r="13" spans="10:22" x14ac:dyDescent="0.2">
+    <row r="13" spans="10:22" x14ac:dyDescent="0.25">
       <c r="J13" t="s">
         <v>112</v>
       </c>
@@ -6462,12 +7112,12 @@
         <v>17306.25</v>
       </c>
     </row>
-    <row r="14" spans="10:22" x14ac:dyDescent="0.2">
+    <row r="14" spans="10:22" x14ac:dyDescent="0.25">
       <c r="J14" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="16" spans="10:22" x14ac:dyDescent="0.2">
+    <row r="16" spans="10:22" x14ac:dyDescent="0.25">
       <c r="J16" t="s">
         <v>114</v>
       </c>
@@ -6475,26 +7125,26 @@
         <v>134</v>
       </c>
     </row>
-    <row r="17" spans="10:23" x14ac:dyDescent="0.2">
+    <row r="17" spans="10:23" x14ac:dyDescent="0.25">
       <c r="J17" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="18" spans="10:23" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="10:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J18" t="s">
         <v>116</v>
       </c>
-      <c r="Q18" s="45" t="s">
+      <c r="Q18" s="49" t="s">
         <v>135</v>
       </c>
-      <c r="R18" s="45"/>
-      <c r="S18" s="45"/>
-      <c r="T18" s="45"/>
-      <c r="U18" s="45"/>
-      <c r="V18" s="45"/>
-      <c r="W18" s="45"/>
-    </row>
-    <row r="19" spans="10:23" x14ac:dyDescent="0.2">
+      <c r="R18" s="49"/>
+      <c r="S18" s="49"/>
+      <c r="T18" s="49"/>
+      <c r="U18" s="49"/>
+      <c r="V18" s="49"/>
+      <c r="W18" s="49"/>
+    </row>
+    <row r="19" spans="10:23" x14ac:dyDescent="0.25">
       <c r="Q19" s="2" t="s">
         <v>136</v>
       </c>
@@ -6515,12 +7165,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="10:23" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="L20" s="45" t="s">
+    <row r="20" spans="10:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L20" s="49" t="s">
         <v>123</v>
       </c>
-      <c r="M20" s="45"/>
-      <c r="N20" s="45"/>
+      <c r="M20" s="49"/>
+      <c r="N20" s="49"/>
       <c r="Q20" s="2" t="s">
         <v>137</v>
       </c>
@@ -6532,7 +7182,7 @@
         <v>28000</v>
       </c>
     </row>
-    <row r="21" spans="10:23" x14ac:dyDescent="0.2">
+    <row r="21" spans="10:23" x14ac:dyDescent="0.25">
       <c r="J21" t="s">
         <v>117</v>
       </c>
@@ -6550,7 +7200,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="22" spans="10:23" x14ac:dyDescent="0.2">
+    <row r="22" spans="10:23" x14ac:dyDescent="0.25">
       <c r="J22" t="s">
         <v>118</v>
       </c>
@@ -6578,7 +7228,7 @@
         <v>55000</v>
       </c>
     </row>
-    <row r="23" spans="10:23" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="10:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J23" t="s">
         <v>119</v>
       </c>
@@ -6606,7 +7256,7 @@
         <v>-17306.25</v>
       </c>
     </row>
-    <row r="24" spans="10:23" x14ac:dyDescent="0.2">
+    <row r="24" spans="10:23" x14ac:dyDescent="0.25">
       <c r="Q24" s="2" t="s">
         <v>139</v>
       </c>
@@ -6632,7 +7282,7 @@
         <v>75693.75</v>
       </c>
     </row>
-    <row r="25" spans="10:23" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="10:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J25" t="s">
         <v>120</v>
       </c>
@@ -6664,7 +7314,7 @@
         <v>0.63600000000000001</v>
       </c>
     </row>
-    <row r="26" spans="10:23" x14ac:dyDescent="0.2">
+    <row r="26" spans="10:23" x14ac:dyDescent="0.25">
       <c r="J26" t="s">
         <v>119</v>
       </c>
@@ -6697,8 +7347,8 @@
         <v>48141.224999999999</v>
       </c>
     </row>
-    <row r="27" spans="10:23" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="10:23" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="10:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="10:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J28" t="s">
         <v>121</v>
       </c>
@@ -6710,16 +7360,16 @@
       <c r="N28" t="s">
         <v>127</v>
       </c>
-      <c r="Q28" s="43" t="s">
+      <c r="Q28" s="51" t="s">
         <v>90</v>
       </c>
-      <c r="R28" s="44"/>
+      <c r="R28" s="52"/>
       <c r="S28" s="25">
         <f>SUM(S26:W26)</f>
         <v>79128.850000000006</v>
       </c>
     </row>
-    <row r="29" spans="10:23" x14ac:dyDescent="0.2">
+    <row r="29" spans="10:23" x14ac:dyDescent="0.25">
       <c r="J29" t="s">
         <v>119</v>
       </c>
@@ -6728,12 +7378,12 @@
         <v>25312.5</v>
       </c>
     </row>
-    <row r="30" spans="10:23" x14ac:dyDescent="0.2">
+    <row r="30" spans="10:23" x14ac:dyDescent="0.25">
       <c r="Q30" s="15" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="31" spans="10:23" x14ac:dyDescent="0.2">
+    <row r="31" spans="10:23" x14ac:dyDescent="0.25">
       <c r="J31" t="s">
         <v>126</v>
       </c>
@@ -6748,7 +7398,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="32" spans="10:23" x14ac:dyDescent="0.2">
+    <row r="32" spans="10:23" x14ac:dyDescent="0.25">
       <c r="J32" s="2" t="s">
         <v>122</v>
       </c>
@@ -6761,20 +7411,20 @@
         <v>144</v>
       </c>
     </row>
-    <row r="33" spans="10:23" x14ac:dyDescent="0.2">
+    <row r="33" spans="10:23" x14ac:dyDescent="0.25">
       <c r="Q33" s="15" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="34" spans="10:23" x14ac:dyDescent="0.2">
+    <row r="34" spans="10:23" x14ac:dyDescent="0.25">
       <c r="Q34" s="15" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="35" spans="10:23" ht="17" x14ac:dyDescent="0.25">
+    <row r="35" spans="10:23" ht="15.75" x14ac:dyDescent="0.25">
       <c r="Q35" s="3"/>
     </row>
-    <row r="36" spans="10:23" x14ac:dyDescent="0.2">
+    <row r="36" spans="10:23" x14ac:dyDescent="0.25">
       <c r="J36" s="2" t="s">
         <v>17</v>
       </c>
@@ -6782,36 +7432,36 @@
         <v>154</v>
       </c>
     </row>
-    <row r="37" spans="10:23" x14ac:dyDescent="0.2">
+    <row r="37" spans="10:23" x14ac:dyDescent="0.25">
       <c r="Q37" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="38" spans="10:23" x14ac:dyDescent="0.2">
+    <row r="38" spans="10:23" x14ac:dyDescent="0.25">
       <c r="J38" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="39" spans="10:23" x14ac:dyDescent="0.2">
+    <row r="39" spans="10:23" x14ac:dyDescent="0.25">
       <c r="J39" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="40" spans="10:23" x14ac:dyDescent="0.2">
+    <row r="40" spans="10:23" x14ac:dyDescent="0.25">
       <c r="J40" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="42" spans="10:23" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J42" s="45" t="s">
+    <row r="42" spans="10:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J42" s="49" t="s">
         <v>90</v>
       </c>
-      <c r="K42" s="45"/>
+      <c r="K42" s="49"/>
       <c r="N42" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="43" spans="10:23" x14ac:dyDescent="0.2">
+    <row r="43" spans="10:23" x14ac:dyDescent="0.25">
       <c r="J43" s="26">
         <v>0.1</v>
       </c>
@@ -6822,7 +7472,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="44" spans="10:23" x14ac:dyDescent="0.2">
+    <row r="44" spans="10:23" x14ac:dyDescent="0.25">
       <c r="J44" s="26">
         <v>0.2</v>
       </c>
@@ -6833,22 +7483,22 @@
         <v>153</v>
       </c>
     </row>
-    <row r="45" spans="10:23" x14ac:dyDescent="0.2">
+    <row r="45" spans="10:23" x14ac:dyDescent="0.25">
       <c r="J45" s="27">
         <v>0.25</v>
       </c>
       <c r="K45" s="2">
         <v>646</v>
       </c>
-      <c r="L45" s="46" t="s">
+      <c r="L45" s="53" t="s">
         <v>150</v>
       </c>
-      <c r="M45" s="46"/>
+      <c r="M45" s="53"/>
       <c r="Q45" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="46" spans="10:23" x14ac:dyDescent="0.2">
+    <row r="46" spans="10:23" x14ac:dyDescent="0.25">
       <c r="J46" s="26">
         <v>0.3</v>
       </c>
@@ -6859,7 +7509,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="47" spans="10:23" x14ac:dyDescent="0.2">
+    <row r="47" spans="10:23" x14ac:dyDescent="0.25">
       <c r="J47" s="26">
         <v>0.6</v>
       </c>
@@ -6870,7 +7520,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="48" spans="10:23" x14ac:dyDescent="0.2">
+    <row r="48" spans="10:23" x14ac:dyDescent="0.25">
       <c r="J48" s="26">
         <v>1.5</v>
       </c>
@@ -6882,7 +7532,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="49" spans="10:23" x14ac:dyDescent="0.2">
+    <row r="49" spans="10:23" x14ac:dyDescent="0.25">
       <c r="J49" s="26">
         <v>2</v>
       </c>
@@ -6890,7 +7540,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="50" spans="10:23" x14ac:dyDescent="0.2">
+    <row r="50" spans="10:23" x14ac:dyDescent="0.25">
       <c r="J50" s="26">
         <v>3</v>
       </c>
@@ -6898,12 +7548,12 @@
         <v>-74</v>
       </c>
     </row>
-    <row r="52" spans="10:23" x14ac:dyDescent="0.2">
+    <row r="52" spans="10:23" x14ac:dyDescent="0.25">
       <c r="J52" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="53" spans="10:23" x14ac:dyDescent="0.2">
+    <row r="53" spans="10:23" x14ac:dyDescent="0.25">
       <c r="J53" t="s">
         <v>164</v>
       </c>
@@ -6911,7 +7561,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="54" spans="10:23" x14ac:dyDescent="0.2">
+    <row r="54" spans="10:23" x14ac:dyDescent="0.25">
       <c r="J54" t="s">
         <v>165</v>
       </c>
@@ -6919,18 +7569,18 @@
         <v>161</v>
       </c>
     </row>
-    <row r="55" spans="10:23" x14ac:dyDescent="0.2">
+    <row r="55" spans="10:23" x14ac:dyDescent="0.25">
       <c r="W55" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="56" spans="10:23" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J56" s="45" t="s">
+    <row r="56" spans="10:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J56" s="49" t="s">
         <v>90</v>
       </c>
-      <c r="K56" s="45"/>
-    </row>
-    <row r="57" spans="10:23" x14ac:dyDescent="0.2">
+      <c r="K56" s="49"/>
+    </row>
+    <row r="57" spans="10:23" x14ac:dyDescent="0.25">
       <c r="J57" s="26">
         <v>0.1</v>
       </c>
@@ -6938,7 +7588,7 @@
         <v>-314</v>
       </c>
     </row>
-    <row r="58" spans="10:23" x14ac:dyDescent="0.2">
+    <row r="58" spans="10:23" x14ac:dyDescent="0.25">
       <c r="J58" s="26">
         <v>0.2</v>
       </c>
@@ -6946,19 +7596,19 @@
         <v>-222</v>
       </c>
     </row>
-    <row r="59" spans="10:23" x14ac:dyDescent="0.2">
+    <row r="59" spans="10:23" x14ac:dyDescent="0.25">
       <c r="J59" s="27">
         <v>0.25</v>
       </c>
       <c r="K59" s="2">
         <v>-200</v>
       </c>
-      <c r="L59" s="46" t="s">
+      <c r="L59" s="53" t="s">
         <v>166</v>
       </c>
-      <c r="M59" s="46"/>
-    </row>
-    <row r="60" spans="10:23" x14ac:dyDescent="0.2">
+      <c r="M59" s="53"/>
+    </row>
+    <row r="60" spans="10:23" x14ac:dyDescent="0.25">
       <c r="J60" s="26">
         <v>0.3</v>
       </c>
@@ -6966,7 +7616,7 @@
         <v>-189</v>
       </c>
     </row>
-    <row r="61" spans="10:23" x14ac:dyDescent="0.2">
+    <row r="61" spans="10:23" x14ac:dyDescent="0.25">
       <c r="J61" s="26">
         <v>0.4</v>
       </c>
@@ -6974,33 +7624,33 @@
         <v>-193</v>
       </c>
     </row>
-    <row r="63" spans="10:23" x14ac:dyDescent="0.2">
+    <row r="63" spans="10:23" x14ac:dyDescent="0.25">
       <c r="J63" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="64" spans="10:23" x14ac:dyDescent="0.2">
+    <row r="64" spans="10:23" x14ac:dyDescent="0.25">
       <c r="J64" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="65" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="65" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J65" t="s">
         <v>169</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="Q28:R28"/>
+    <mergeCell ref="J42:K42"/>
+    <mergeCell ref="L45:M45"/>
+    <mergeCell ref="J56:K56"/>
+    <mergeCell ref="L59:M59"/>
     <mergeCell ref="J6:M6"/>
     <mergeCell ref="L20:N20"/>
     <mergeCell ref="Q6:V6"/>
     <mergeCell ref="Q10:R11"/>
     <mergeCell ref="Q18:W18"/>
-    <mergeCell ref="Q28:R28"/>
-    <mergeCell ref="J42:K42"/>
-    <mergeCell ref="L45:M45"/>
-    <mergeCell ref="J56:K56"/>
-    <mergeCell ref="L59:M59"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -7018,18 +7668,18 @@
       <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="11" max="11" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="10:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="10:18" x14ac:dyDescent="0.25">
       <c r="J1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="10:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="10:18" x14ac:dyDescent="0.25">
       <c r="J3" s="2" t="s">
         <v>170</v>
       </c>
@@ -7037,12 +7687,12 @@
         <v>178</v>
       </c>
     </row>
-    <row r="4" spans="10:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="10:18" x14ac:dyDescent="0.25">
       <c r="O4" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="5" spans="10:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="10:18" x14ac:dyDescent="0.25">
       <c r="J5" t="s">
         <v>136</v>
       </c>
@@ -7056,7 +7706,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="6" spans="10:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="10:18" x14ac:dyDescent="0.25">
       <c r="J6" t="s">
         <v>117</v>
       </c>
@@ -7067,7 +7717,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="7" spans="10:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="10:18" x14ac:dyDescent="0.25">
       <c r="J7" t="s">
         <v>171</v>
       </c>
@@ -7078,7 +7728,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="8" spans="10:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="10:18" x14ac:dyDescent="0.25">
       <c r="J8" t="s">
         <v>172</v>
       </c>
@@ -7089,7 +7739,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="9" spans="10:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="10:18" x14ac:dyDescent="0.25">
       <c r="J9" t="s">
         <v>70</v>
       </c>
@@ -7102,17 +7752,17 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="10:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="10:18" x14ac:dyDescent="0.25">
       <c r="O10" s="2" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="11" spans="10:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="10:18" x14ac:dyDescent="0.25">
       <c r="J11" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="12" spans="10:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="10:18" x14ac:dyDescent="0.25">
       <c r="O12" t="s">
         <v>185</v>
       </c>
@@ -7120,7 +7770,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="13" spans="10:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="10:18" x14ac:dyDescent="0.25">
       <c r="O13" t="s">
         <v>186</v>
       </c>
@@ -7128,7 +7778,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="14" spans="10:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="10:18" x14ac:dyDescent="0.25">
       <c r="J14" s="2" t="s">
         <v>174</v>
       </c>
@@ -7139,7 +7789,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="16" spans="10:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="10:18" x14ac:dyDescent="0.25">
       <c r="J16" t="s">
         <v>136</v>
       </c>
@@ -7156,7 +7806,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="17" spans="10:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="10:16" x14ac:dyDescent="0.25">
       <c r="J17" t="s">
         <v>117</v>
       </c>
@@ -7167,7 +7817,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="18" spans="10:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="10:16" x14ac:dyDescent="0.25">
       <c r="J18" t="s">
         <v>171</v>
       </c>
@@ -7178,7 +7828,7 @@
         <v>-6000</v>
       </c>
     </row>
-    <row r="19" spans="10:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="10:16" x14ac:dyDescent="0.25">
       <c r="J19" t="s">
         <v>172</v>
       </c>
@@ -7187,7 +7837,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="20" spans="10:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="10:16" x14ac:dyDescent="0.25">
       <c r="J20" t="s">
         <v>70</v>
       </c>
@@ -7204,17 +7854,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="10:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="10:16" x14ac:dyDescent="0.25">
       <c r="J22" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="25" spans="10:16" x14ac:dyDescent="0.2">
+    <row r="25" spans="10:16" x14ac:dyDescent="0.25">
       <c r="J25" s="2" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="27" spans="10:16" x14ac:dyDescent="0.2">
+    <row r="27" spans="10:16" x14ac:dyDescent="0.25">
       <c r="J27" t="s">
         <v>136</v>
       </c>
@@ -7231,7 +7881,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="10:16" x14ac:dyDescent="0.2">
+    <row r="28" spans="10:16" x14ac:dyDescent="0.25">
       <c r="J28" t="s">
         <v>117</v>
       </c>
@@ -7239,7 +7889,7 @@
         <v>-12000</v>
       </c>
     </row>
-    <row r="29" spans="10:16" x14ac:dyDescent="0.2">
+    <row r="29" spans="10:16" x14ac:dyDescent="0.25">
       <c r="J29" t="s">
         <v>171</v>
       </c>
@@ -7253,7 +7903,7 @@
         <v>-8000</v>
       </c>
     </row>
-    <row r="30" spans="10:16" x14ac:dyDescent="0.2">
+    <row r="30" spans="10:16" x14ac:dyDescent="0.25">
       <c r="J30" t="s">
         <v>172</v>
       </c>
@@ -7263,7 +7913,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="31" spans="10:16" x14ac:dyDescent="0.2">
+    <row r="31" spans="10:16" x14ac:dyDescent="0.25">
       <c r="J31" t="s">
         <v>70</v>
       </c>
@@ -7284,27 +7934,27 @@
         <v>-5000</v>
       </c>
     </row>
-    <row r="33" spans="10:16" x14ac:dyDescent="0.2">
+    <row r="33" spans="10:16" x14ac:dyDescent="0.25">
       <c r="J33" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="36" spans="10:16" x14ac:dyDescent="0.2">
+    <row r="36" spans="10:16" x14ac:dyDescent="0.25">
       <c r="J36" s="2" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="38" spans="10:16" x14ac:dyDescent="0.2">
+    <row r="38" spans="10:16" x14ac:dyDescent="0.25">
       <c r="J38" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="39" spans="10:16" x14ac:dyDescent="0.2">
+    <row r="39" spans="10:16" x14ac:dyDescent="0.25">
       <c r="J39" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="42" spans="10:16" x14ac:dyDescent="0.2">
+    <row r="42" spans="10:16" x14ac:dyDescent="0.25">
       <c r="J42" s="2" t="s">
         <v>196</v>
       </c>
@@ -7324,7 +7974,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="43" spans="10:16" x14ac:dyDescent="0.2">
+    <row r="43" spans="10:16" x14ac:dyDescent="0.25">
       <c r="J43" s="2" t="s">
         <v>200</v>
       </c>
@@ -7346,7 +7996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="10:16" x14ac:dyDescent="0.2">
+    <row r="44" spans="10:16" x14ac:dyDescent="0.25">
       <c r="J44" s="2" t="s">
         <v>201</v>
       </c>
@@ -7368,7 +8018,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="45" spans="10:16" x14ac:dyDescent="0.2">
+    <row r="45" spans="10:16" x14ac:dyDescent="0.25">
       <c r="J45" s="2" t="s">
         <v>202</v>
       </c>
@@ -7390,7 +8040,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="10:16" x14ac:dyDescent="0.2">
+    <row r="46" spans="10:16" x14ac:dyDescent="0.25">
       <c r="J46" s="2" t="s">
         <v>203</v>
       </c>
@@ -7412,7 +8062,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="10:16" x14ac:dyDescent="0.2">
+    <row r="47" spans="10:16" x14ac:dyDescent="0.25">
       <c r="J47" s="2" t="s">
         <v>204</v>
       </c>
@@ -7434,7 +8084,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="J49" s="2" t="s">
         <v>196</v>
       </c>
@@ -7448,7 +8098,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="J50" s="2" t="s">
         <v>200</v>
       </c>
@@ -7463,7 +8113,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="J51" s="2" t="s">
         <v>203</v>
       </c>
@@ -7478,7 +8128,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>216</v>
       </c>
@@ -7498,7 +8148,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="J53" s="2" t="s">
         <v>208</v>
       </c>
@@ -7514,7 +8164,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>217</v>
       </c>
@@ -7522,32 +8172,32 @@
         <v>215</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>223</v>
       </c>
@@ -7569,14 +8219,14 @@
       <selection activeCell="J41" sqref="J41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="10:22" x14ac:dyDescent="0.2">
+    <row r="2" spans="10:22" x14ac:dyDescent="0.25">
       <c r="J2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="10:22" x14ac:dyDescent="0.2">
+    <row r="4" spans="10:22" x14ac:dyDescent="0.25">
       <c r="J4" s="2" t="s">
         <v>228</v>
       </c>
@@ -7584,7 +8234,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="6" spans="10:22" x14ac:dyDescent="0.2">
+    <row r="6" spans="10:22" x14ac:dyDescent="0.25">
       <c r="J6" s="40"/>
       <c r="K6" s="39"/>
       <c r="L6" s="12" t="s">
@@ -7614,7 +8264,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="10:22" x14ac:dyDescent="0.2">
+    <row r="7" spans="10:22" x14ac:dyDescent="0.25">
       <c r="J7" s="33" t="s">
         <v>197</v>
       </c>
@@ -7632,7 +8282,7 @@
       </c>
       <c r="V7" s="18"/>
     </row>
-    <row r="8" spans="10:22" x14ac:dyDescent="0.2">
+    <row r="8" spans="10:22" x14ac:dyDescent="0.25">
       <c r="J8" s="33" t="s">
         <v>138</v>
       </c>
@@ -7654,7 +8304,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="9" spans="10:22" x14ac:dyDescent="0.2">
+    <row r="9" spans="10:22" x14ac:dyDescent="0.25">
       <c r="J9" s="33" t="s">
         <v>108</v>
       </c>
@@ -7682,7 +8332,7 @@
         <v>205000</v>
       </c>
     </row>
-    <row r="10" spans="10:22" x14ac:dyDescent="0.2">
+    <row r="10" spans="10:22" x14ac:dyDescent="0.25">
       <c r="J10" s="33" t="s">
         <v>224</v>
       </c>
@@ -7710,7 +8360,7 @@
         <v>-50000</v>
       </c>
     </row>
-    <row r="11" spans="10:22" x14ac:dyDescent="0.2">
+    <row r="11" spans="10:22" x14ac:dyDescent="0.25">
       <c r="J11" s="33" t="s">
         <v>225</v>
       </c>
@@ -7738,7 +8388,7 @@
         <v>-75000</v>
       </c>
     </row>
-    <row r="12" spans="10:22" x14ac:dyDescent="0.2">
+    <row r="12" spans="10:22" x14ac:dyDescent="0.25">
       <c r="J12" s="33" t="s">
         <v>226</v>
       </c>
@@ -7768,7 +8418,7 @@
         <v>-6000</v>
       </c>
     </row>
-    <row r="13" spans="10:22" x14ac:dyDescent="0.2">
+    <row r="13" spans="10:22" x14ac:dyDescent="0.25">
       <c r="J13" s="33" t="s">
         <v>70</v>
       </c>
@@ -7810,7 +8460,7 @@
         <v>94000</v>
       </c>
     </row>
-    <row r="14" spans="10:22" x14ac:dyDescent="0.2">
+    <row r="14" spans="10:22" x14ac:dyDescent="0.25">
       <c r="J14" s="33" t="s">
         <v>140</v>
       </c>
@@ -7844,7 +8494,7 @@
         <v>0.751</v>
       </c>
     </row>
-    <row r="15" spans="10:22" x14ac:dyDescent="0.2">
+    <row r="15" spans="10:22" x14ac:dyDescent="0.25">
       <c r="J15" s="33" t="s">
         <v>227</v>
       </c>
@@ -7886,7 +8536,7 @@
         <v>70594</v>
       </c>
     </row>
-    <row r="16" spans="10:22" x14ac:dyDescent="0.2">
+    <row r="16" spans="10:22" x14ac:dyDescent="0.25">
       <c r="J16" s="37" t="s">
         <v>90</v>
       </c>
@@ -7910,22 +8560,22 @@
       <c r="U16" s="9"/>
       <c r="V16" s="38"/>
     </row>
-    <row r="18" spans="10:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="10:14" x14ac:dyDescent="0.25">
       <c r="J18" s="2" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="19" spans="10:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="10:14" x14ac:dyDescent="0.25">
       <c r="J19" s="2" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="22" spans="10:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="10:14" x14ac:dyDescent="0.25">
       <c r="J22" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="10:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="10:14" x14ac:dyDescent="0.25">
       <c r="J24" s="2" t="s">
         <v>193</v>
       </c>
@@ -7933,7 +8583,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="26" spans="10:14" x14ac:dyDescent="0.2">
+    <row r="26" spans="10:14" x14ac:dyDescent="0.25">
       <c r="J26" s="2" t="s">
         <v>232</v>
       </c>
@@ -7941,7 +8591,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="27" spans="10:14" x14ac:dyDescent="0.2">
+    <row r="27" spans="10:14" x14ac:dyDescent="0.25">
       <c r="J27" t="s">
         <v>233</v>
       </c>
@@ -7949,62 +8599,62 @@
         <v>245</v>
       </c>
     </row>
-    <row r="28" spans="10:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="10:14" x14ac:dyDescent="0.25">
       <c r="J28" s="1" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="29" spans="10:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="10:14" x14ac:dyDescent="0.25">
       <c r="N29" s="2" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="30" spans="10:14" x14ac:dyDescent="0.2">
+    <row r="30" spans="10:14" x14ac:dyDescent="0.25">
       <c r="J30" s="2" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="31" spans="10:14" x14ac:dyDescent="0.2">
+    <row r="31" spans="10:14" x14ac:dyDescent="0.25">
       <c r="J31" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="32" spans="10:14" x14ac:dyDescent="0.2">
+    <row r="32" spans="10:14" x14ac:dyDescent="0.25">
       <c r="J32" s="1" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="34" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J34" s="2" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="35" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J35" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="36" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J36" s="1" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="38" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J38" s="2" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="39" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J39" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="40" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J40" s="1" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="41" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J41" s="41">
         <v>141900</v>
       </c>
@@ -8024,14 +8674,14 @@
       <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="10:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="10:21" x14ac:dyDescent="0.25">
       <c r="J1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="10:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="10:21" x14ac:dyDescent="0.25">
       <c r="J3" s="2" t="s">
         <v>193</v>
       </c>
@@ -8039,7 +8689,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="5" spans="10:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="10:21" x14ac:dyDescent="0.25">
       <c r="J5" t="s">
         <v>247</v>
       </c>
@@ -8047,7 +8697,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="6" spans="10:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="10:21" x14ac:dyDescent="0.25">
       <c r="J6" t="s">
         <v>264</v>
       </c>
@@ -8055,7 +8705,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="7" spans="10:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="10:21" x14ac:dyDescent="0.25">
       <c r="J7" t="s">
         <v>248</v>
       </c>
@@ -8063,12 +8713,12 @@
         <v>269</v>
       </c>
     </row>
-    <row r="8" spans="10:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="10:21" x14ac:dyDescent="0.25">
       <c r="J8" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="9" spans="10:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="10:21" x14ac:dyDescent="0.25">
       <c r="J9" t="s">
         <v>249</v>
       </c>
@@ -8076,17 +8726,17 @@
         <v>270</v>
       </c>
     </row>
-    <row r="10" spans="10:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="10:21" x14ac:dyDescent="0.25">
       <c r="S10" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="11" spans="10:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="10:21" x14ac:dyDescent="0.25">
       <c r="J11" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="12" spans="10:21" x14ac:dyDescent="0.2">
+    <row r="12" spans="10:21" x14ac:dyDescent="0.25">
       <c r="J12" t="s">
         <v>251</v>
       </c>
@@ -8094,7 +8744,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="13" spans="10:21" x14ac:dyDescent="0.2">
+    <row r="13" spans="10:21" x14ac:dyDescent="0.25">
       <c r="J13" t="s">
         <v>252</v>
       </c>
@@ -8102,7 +8752,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="14" spans="10:21" x14ac:dyDescent="0.2">
+    <row r="14" spans="10:21" x14ac:dyDescent="0.25">
       <c r="J14" t="s">
         <v>253</v>
       </c>
@@ -8116,7 +8766,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="16" spans="10:21" x14ac:dyDescent="0.2">
+    <row r="16" spans="10:21" x14ac:dyDescent="0.25">
       <c r="J16" t="s">
         <v>254</v>
       </c>
@@ -8124,7 +8774,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="J17" t="s">
         <v>255</v>
       </c>
@@ -8132,7 +8782,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="J18" t="s">
         <v>256</v>
       </c>
@@ -8140,12 +8790,12 @@
         <v>277</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="J19" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="J20" t="s">
         <v>258</v>
       </c>
@@ -8153,7 +8803,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>285</v>
       </c>
@@ -8164,7 +8814,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>286</v>
       </c>
@@ -8175,7 +8825,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="J24" t="s">
         <v>260</v>
       </c>
@@ -8183,7 +8833,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>287</v>
       </c>
@@ -8200,12 +8850,12 @@
         <v>282</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="J26" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>288</v>
       </c>
@@ -8213,7 +8863,7 @@
         <v>13510</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>289</v>
       </c>
@@ -8224,7 +8874,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>208</v>
       </c>
@@ -8233,12 +8883,12 @@
         <v>13510</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>291</v>
       </c>
@@ -8246,7 +8896,7 @@
         <v>11580</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>292</v>
       </c>
@@ -8254,7 +8904,7 @@
         <v>1920</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>208</v>
       </c>
@@ -8263,17 +8913,17 @@
         <v>13500</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>295</v>
       </c>
@@ -8281,7 +8931,7 @@
         <v>12545</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>296</v>
       </c>
@@ -8289,7 +8939,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>208</v>
       </c>
@@ -8298,12 +8948,12 @@
         <v>13505</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>298</v>
       </c>
@@ -8311,7 +8961,7 @@
         <v>11580</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>299</v>
       </c>
@@ -8319,7 +8969,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>208</v>
       </c>
@@ -8342,59 +8992,59 @@
       <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J4" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="5" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J5" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="8" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J8" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J10" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="11" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J11" s="2" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="12" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J12" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="13" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J13" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="16" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J16" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="10:18" x14ac:dyDescent="0.2">
+    <row r="17" spans="10:18" x14ac:dyDescent="0.25">
       <c r="J17" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="19" spans="10:18" x14ac:dyDescent="0.2">
+    <row r="19" spans="10:18" x14ac:dyDescent="0.25">
       <c r="J19" s="2" t="s">
         <v>307</v>
       </c>
@@ -8402,7 +9052,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="20" spans="10:18" x14ac:dyDescent="0.2">
+    <row r="20" spans="10:18" x14ac:dyDescent="0.25">
       <c r="J20" t="s">
         <v>308</v>
       </c>
@@ -8410,7 +9060,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="21" spans="10:18" x14ac:dyDescent="0.2">
+    <row r="21" spans="10:18" x14ac:dyDescent="0.25">
       <c r="J21" t="s">
         <v>309</v>
       </c>
@@ -8418,7 +9068,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="22" spans="10:18" x14ac:dyDescent="0.2">
+    <row r="22" spans="10:18" x14ac:dyDescent="0.25">
       <c r="J22" t="s">
         <v>310</v>
       </c>
@@ -8426,7 +9076,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="23" spans="10:18" x14ac:dyDescent="0.2">
+    <row r="23" spans="10:18" x14ac:dyDescent="0.25">
       <c r="J23" t="s">
         <v>311</v>
       </c>
@@ -8434,7 +9084,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="24" spans="10:18" x14ac:dyDescent="0.2">
+    <row r="24" spans="10:18" x14ac:dyDescent="0.25">
       <c r="J24" t="s">
         <v>312</v>
       </c>
@@ -8442,7 +9092,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="25" spans="10:18" x14ac:dyDescent="0.2">
+    <row r="25" spans="10:18" x14ac:dyDescent="0.25">
       <c r="J25" t="s">
         <v>313</v>
       </c>
@@ -8450,12 +9100,12 @@
         <v>320</v>
       </c>
     </row>
-    <row r="26" spans="10:18" x14ac:dyDescent="0.2">
+    <row r="26" spans="10:18" x14ac:dyDescent="0.25">
       <c r="R26" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="27" spans="10:18" x14ac:dyDescent="0.2">
+    <row r="27" spans="10:18" x14ac:dyDescent="0.25">
       <c r="J27" t="s">
         <v>328</v>
       </c>
@@ -8463,7 +9113,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="28" spans="10:18" x14ac:dyDescent="0.2">
+    <row r="28" spans="10:18" x14ac:dyDescent="0.25">
       <c r="J28" t="s">
         <v>329</v>
       </c>
@@ -8471,17 +9121,17 @@
         <v>323</v>
       </c>
     </row>
-    <row r="29" spans="10:18" x14ac:dyDescent="0.2">
+    <row r="29" spans="10:18" x14ac:dyDescent="0.25">
       <c r="R29" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="30" spans="10:18" x14ac:dyDescent="0.2">
+    <row r="30" spans="10:18" x14ac:dyDescent="0.25">
       <c r="R30" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="31" spans="10:18" x14ac:dyDescent="0.2">
+    <row r="31" spans="10:18" x14ac:dyDescent="0.25">
       <c r="J31" s="2" t="s">
         <v>347</v>
       </c>
@@ -8489,7 +9139,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="32" spans="10:18" x14ac:dyDescent="0.2">
+    <row r="32" spans="10:18" x14ac:dyDescent="0.25">
       <c r="J32" t="s">
         <v>345</v>
       </c>
@@ -8497,82 +9147,82 @@
         <v>327</v>
       </c>
     </row>
-    <row r="33" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J33" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="34" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J34" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="35" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J35" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="36" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J36" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="37" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J37" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="38" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J38" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="39" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J39" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="41" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J41" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="42" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J42" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="43" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J43" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="44" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J44" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="45" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J45" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="46" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J46" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="47" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J47" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="48" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J48" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="49" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="49" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J49" t="s">
         <v>344</v>
       </c>
@@ -8591,7 +9241,7 @@
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -8604,7 +9254,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8619,15 +9269,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B115D461E3186840B6295614C3F6CBF7" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="36c5d3abd2f5f65b7e4df3c95a7fac60">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="fc68bb02-cea7-47a7-8486-5fa5775c5400" xmlns:ns4="9ad45b7a-dbde-452b-a4a7-7cb6f25a272a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="19f510c93a1a7c10f8de96c2513e45d1" ns3:_="" ns4:_="">
     <xsd:import namespace="fc68bb02-cea7-47a7-8486-5fa5775c5400"/>
@@ -8846,6 +9487,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E46C5FB1-8F9C-4831-826C-7C1683BB76AE}">
   <ds:schemaRefs>
@@ -8864,14 +9514,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF5FFC30-E5CB-4FF2-BD48-577C518BCEE5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{27D7E961-E2C3-4250-962F-5198B7DAE13D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8890,6 +9532,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF5FFC30-E5CB-4FF2-BD48-577C518BCEE5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{b52e9fda-0691-4585-bdfc-5ccae1ce1890}" enabled="0" method="" siteId="{b52e9fda-0691-4585-bdfc-5ccae1ce1890}" removed="1"/>

</xml_diff>